<commit_message>
feat: update prototype with esp32
</commit_message>
<xml_diff>
--- a/simulation/Specifications.xlsx
+++ b/simulation/Specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Github\Horizon\simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9162698A-E067-4ADC-BA95-9101B5CC055B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1F35C2-4D9E-4DE2-AC36-455925CAA493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F2ED7FED-07B8-453D-A522-43D245FF19C0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F2ED7FED-07B8-453D-A522-43D245FF19C0}"/>
   </bookViews>
   <sheets>
     <sheet name="EMAX-MT2213" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -116,7 +116,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,12 +173,20 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Profile</a:t>
+              <a:t> Thrust Profile</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39305084886631914"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -229,10 +237,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -252,40 +258,95 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.1416649424399916E-2"/>
+                  <c:y val="0.12516149023038786"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'EMAX-MT2213'!$A$2:$A$11</c:f>
+              <c:f>'EMAX-MT2213'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>9.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -293,38 +354,41 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'EMAX-MT2213'!$B$2:$B$11</c:f>
+              <c:f>'EMAX-MT2213'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>290</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>490</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>540</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>620</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
@@ -337,25 +401,377 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="147525759"/>
+        <c:axId val="147522879"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="147525759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="147522879"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="147522879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="147525759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Motor</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> RPM Profile</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39305084886631914"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="3"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'EMAX-MT2213'!$C$1</c:f>
+              <c:f>'EMAX-MT2213'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Power (W)</c:v>
+                  <c:v>Speed (RPM)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -365,50 +781,105 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.6529418223318928E-4"/>
+                  <c:y val="0.16682815689705455"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'EMAX-MT2213'!$A$2:$A$11</c:f>
+              <c:f>'EMAX-MT2213'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>9.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -416,39 +887,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'EMAX-MT2213'!$C$2:$C$11</c:f>
+              <c:f>'EMAX-MT2213'!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>2940</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>3860</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>4940</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66</c:v>
+                  <c:v>5340</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>77</c:v>
+                  <c:v>5720</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>88</c:v>
+                  <c:v>5980</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>99</c:v>
+                  <c:v>6170</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>105.5</c:v>
+                  <c:v>6410</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6530</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,7 +930,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E8CE-4CCE-879A-D60660412411}"/>
+              <c16:uniqueId val="{00000004-4748-42D5-A1B0-F00511D5197A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -766,6 +1240,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1282,20 +1796,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>24320</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>25863</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5734</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>86265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>335723</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>102063</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>284612</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>162465</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1315,6 +2345,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>278878</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42FB9BBC-FB49-449F-AD6F-20DFAC6C3ADA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1640,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91CDD898-1F73-4443-B4CC-5FEA1746DF9B}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,186 +2742,201 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="B2" s="1">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2">
-        <f>B2/C2</f>
-        <v>11.818181818181818</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="1">
-        <v>2940</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="C3" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D11" si="0">B3/C3</f>
-        <v>10</v>
+        <f>B3/C3</f>
+        <v>11.818181818181818</v>
       </c>
       <c r="E3" s="1">
-        <v>3860</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>290</v>
+        <v>220</v>
       </c>
       <c r="C4" s="1">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
-        <v>8.7878787878787872</v>
+        <f t="shared" ref="D4:D12" si="0">B4/C4</f>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
-        <v>4400</v>
+        <v>3860</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>360</v>
+        <v>290</v>
       </c>
       <c r="C5" s="1">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>8.1818181818181817</v>
+        <v>8.7878787878787872</v>
       </c>
       <c r="E5" s="1">
-        <v>4940</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>430</v>
+        <v>360</v>
       </c>
       <c r="C6" s="1">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>7.8181818181818183</v>
+        <v>8.1818181818181817</v>
       </c>
       <c r="E6" s="1">
-        <v>5340</v>
+        <v>4940</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>490</v>
+        <v>430</v>
       </c>
       <c r="C7" s="1">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>7.4242424242424239</v>
+        <v>7.8181818181818183</v>
       </c>
       <c r="E7" s="1">
-        <v>5720</v>
+        <v>5340</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>540</v>
+        <v>490</v>
       </c>
       <c r="C8" s="1">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>7.0129870129870131</v>
+        <v>7.4242424242424239</v>
       </c>
       <c r="E8" s="1">
-        <v>5980</v>
+        <v>5720</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="C9" s="1">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>6.5909090909090908</v>
+        <v>7.0129870129870131</v>
       </c>
       <c r="E9" s="1">
-        <v>6170</v>
+        <v>5980</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>620</v>
+        <v>580</v>
       </c>
       <c r="C10" s="1">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>6.262626262626263</v>
+        <v>6.5909090909090908</v>
       </c>
       <c r="E10" s="1">
-        <v>6410</v>
+        <v>6170</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>640</v>
+        <v>620</v>
       </c>
       <c r="C11" s="1">
-        <v>105.5</v>
+        <v>99</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
+        <v>6.262626262626263</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6410</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>640</v>
+      </c>
+      <c r="C12" s="1">
+        <v>105.5</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
         <v>6.0663507109004735</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>6530</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>